<commit_message>
win/linux path issue resolved
</commit_message>
<xml_diff>
--- a/command_line/crs-output/context_visualized.xlsx
+++ b/command_line/crs-output/context_visualized.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -404,27 +404,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>étude,alertant,l',inefficacité,risques</t>
+          <t>$,$,$,$,Loin</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>les risques de</t>
+          <t>$ Loin de</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>certains traitements</t>
+          <t>leurs proches</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>de le Covid-19</t>
+          <t>, coincés dans</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Covid-19,l',hydroxychloroquine,,</t>
+          <t>,,coincés,petites,chambres</t>
         </is>
       </c>
     </row>
@@ -434,27 +434,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>qu',l',analyse,propose,48h</t>
+          <t>étudiant,,,allés,jusqu’,rationner</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>propose sous 48h</t>
+          <t>jusqu’ à rationner</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>une révision</t>
+          <t>leurs repas</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>de les règles</t>
+          <t>, faute d’</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>règles,dérogatoires,prescription,,</t>
+          <t>,,faute,d’,argent</t>
         </is>
       </c>
     </row>
@@ -464,27 +464,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>étude,alertant,l',inefficacité,risques</t>
+          <t>d',outre-mer,,,,,jour</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>les risques de</t>
+          <t>le jour à</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>certains traitements de le Covid-19</t>
+          <t>le lendemain</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>dont l' hydroxychloroquine</t>
+          <t>, dû adapter</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>l',hydroxychloroquine,,,j'</t>
+          <t>,,dû,adapter,quotidien</t>
         </is>
       </c>
     </row>
@@ -494,197 +494,709 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>d',étude,alertant,l',inefficacité</t>
+          <t>mars,2020,gouvernement,français,perdu</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>l' inefficacité et</t>
+          <t>Après avoir perdu</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>les risques</t>
+          <t>leur job étudiant</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>de certains traitements</t>
+          <t>, certains sont</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>traitements,Covid-19,l',hydroxychloroquine</t>
+          <t>,,allés,jusqu’,rationner</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>D’,retrouvés,perspective,stage,d’</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>stage ou d’</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>emploi</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>, sans diplômes</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>,,diplômes,…,sans-papiers</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>,,coincés,petites,chambres,universitaires</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ou dans de</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>les studettes</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>, de les</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>,,milliers,d’,étudiants</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>1</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>risques,traitements,Covid-19,l',hydroxychloroquine</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>dont l' hydroxychloroquine</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>gouvernement,français,perdu,job,étudiant</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>leur job étudiant</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>,</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>j' ai saisi</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>j',saisi,HCSP,qu'</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>certains sont allés</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>allés,jusqu’,rationner,repas</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>1</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>48h,révision,règles,dérogatoires,prescription</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>dérogatoires de prescription</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>retrouvés,perspective,stage,d’,emploi</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ou d’ emploi</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>,</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>a indiqué le</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>indiqué,ministre,tweet,$</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>sans diplômes …</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>diplômes,…,sans-papiers,$</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$,$,$,$,Suite</t>
+          <t>,,milliers,d’,étudiants,étrangers</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$ Suite à</t>
+          <t>d’ étudiants étrangers</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>la publication</t>
+          <t>,</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>dans The Lancet</t>
+          <t>ou venus de</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>The,Lancet,d',étude</t>
+          <t>venus,lointains,départements,d'</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>coincés,petites,chambres,universitaires,studettes</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>de les studettes</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>de les milliers</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>milliers,d’,étudiants,étrangers</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>$,$,$,Loin,proches</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>de leurs proches</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>coincés dans de</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>coincés,petites,chambres,universitaires</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>,,allés,jusqu’,rationner,repas</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>rationner leurs repas</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>faute d’ argent</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>faute,d’,argent,D’</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>outre-mer,,,,,jour,lendemain</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>à le lendemain</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>dû adapter leur</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>dû,adapter,quotidien,face</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>venus,lointains,départements,d',outre-mer</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>départements d' outre-mer</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>ont , de</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>,,jour,lendemain,,</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>lointains,départements,d',outre-mer,,</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>outre-mer , ont</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>de le jour</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>jour,lendemain,,,dû</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>2</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>règles,dérogatoires,prescription,,,indiqué</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>, a indiqué</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>le ministre</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>dans un tweet</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>tweet,$,$,$</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>confinement,imposé,17,mars,2020</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>mars 2020 par</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>le gouvernement français .</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Après avoir perdu</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>perdu,job,étudiant,,</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>face,crise,sanitaire,confinement,imposé</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>le confinement imposé</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>le 17</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>mars 2020 par</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>mars,2020,gouvernement,français</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>face,crise,sanitaire,confinement,imposé</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>le confinement imposé</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>le 17 mars 2020</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>par le gouvernement</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>gouvernement,français,perdu,job</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>confinement,imposé,17,mars,2020</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>mars 2020 par</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>le gouvernement français</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>. Après avoir</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>perdu,job,étudiant,,</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>confinement,imposé,17,mars,2020</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>mars 2020 par</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>le gouvernement</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>français . Après</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>français,perdu,job,étudiant</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>faute,d’,argent,D’,retrouvés</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>sont retrouvés sans</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>perspective de stage</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ou d’ emploi</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>d’,emploi,,,diplômes</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$,Loin,proches,,,coincés</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>, coincés dans</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>de petites chambres universitaires</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>ou dans de</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>studettes,,,milliers,d’</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>emploi,,,diplômes,…,sans-papiers</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>… et sans-papiers</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>$ $ $</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>$,$,$,$</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>repas,,,faute,d’,argent</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>faute d’ argent</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>D’ autres se</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>D’,retrouvés,perspective,stage</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>